<commit_message>
Lesson 17 Updates (no R, no Excel, all by hand)
</commit_message>
<xml_diff>
--- a/docs/Data/Calcium_E2V2.xlsx
+++ b/docs/Data/Calcium_E2V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saharq\OneDrive\Desktop\Desktop\BYU-I\Courses\Math 221B\Exams\Exam 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghsaund/Documents/GitHub/BYUI_M221_Book_R/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{4F8D8C66-2166-4F02-AC7C-B4B40F9A0981}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{A44A35BC-2BDD-4BE1-8B92-D0B3C5969CB2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38AD097-1D8E-AD44-98FB-EE5BFC21E856}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B31A4CDC-AA99-4727-BB98-36A393CEA320}"/>
+    <workbookView xWindow="14540" yWindow="3380" windowWidth="29040" windowHeight="15840" xr2:uid="{B31A4CDC-AA99-4727-BB98-36A393CEA320}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,26 +20,26 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Normal Bone Density</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="5">
   <si>
     <t>Osteopenia</t>
   </si>
   <si>
     <t>Osteoporosis</t>
+  </si>
+  <si>
+    <t>Bone Type</t>
+  </si>
+  <si>
+    <t>Calcium Intake</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
 </sst>
 </file>
@@ -55,34 +55,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9.9"/>
-      <color rgb="FFC00000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9.9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -90,31 +83,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -431,135 +410,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1AA0DC-08EF-44A0-BD55-FFCEB6EDFB06}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
         <v>1200</v>
       </c>
-      <c r="B2" s="2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
         <v>1000</v>
       </c>
-      <c r="C2" s="2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
         <v>890</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
         <v>1000</v>
       </c>
-      <c r="B3" s="2">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
         <v>1100</v>
       </c>
-      <c r="C3" s="2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
         <v>650</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>980</v>
-      </c>
-      <c r="B4" s="2">
-        <v>700</v>
-      </c>
-      <c r="C4" s="2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2">
         <v>1100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2">
         <v>900</v>
       </c>
-      <c r="B5" s="2">
-        <v>800</v>
-      </c>
-      <c r="C5" s="2">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2">
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>750</v>
-      </c>
-      <c r="B6" s="2">
-        <v>500</v>
-      </c>
-      <c r="C6" s="2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>800</v>
-      </c>
-      <c r="B7" s="2">
-        <v>700</v>
-      </c>
-      <c r="C7" s="2">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>920</v>
-      </c>
-      <c r="B8" s="2">
-        <v>750</v>
-      </c>
-      <c r="C8" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>990</v>
-      </c>
-      <c r="B9" s="2">
-        <v>910</v>
-      </c>
-      <c r="C9" s="2">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>890</v>
-      </c>
-      <c r="B10" s="2">
-        <v>680</v>
-      </c>
-      <c r="C10" s="2">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>900</v>
-      </c>
-      <c r="B11" s="2">
-        <v>850</v>
-      </c>
-      <c r="C11" s="2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2">
         <v>640</v>
       </c>
     </row>

</xml_diff>